<commit_message>
Data update from ABS for education participation.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_participation_uploader/education_participation.xlsx
+++ b/dashboard_loader/education_participation_uploader/education_participation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">People who were in school level education are excluded. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">People who were engaged in a combination of education or training and employment, but whose full­time/part-time student status or their full­time/part-time employment status was not identified are included in 'Combination of study and work proportion' and 'Total fully engaged'.</t>
   </si>
   <si>
     <t xml:space="preserve">People permanently unable to work are excluded from the in-scope population.  </t>
@@ -125,7 +128,7 @@
     <numFmt numFmtId="165" formatCode="########\ ###\ ##0.0;\-########\ ###\ ##0.0;\–"/>
     <numFmt numFmtId="166" formatCode="#########\ ###\ ##0.0;\-#########\ ###\ ##0.0;\–"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -150,6 +153,20 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -222,7 +239,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -251,15 +268,23 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -267,11 +292,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -280,6 +305,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,8 +332,8 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -419,39 +448,39 @@
         <v>41.2187585198729</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>2006</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="n">
-        <v>3.80783595535934</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>3.26342427124368</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>3.23995120933993</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>3.10078381851458</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>3.32591483983033</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>2.49637376899</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>5.97562039973235</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>2.62091018100839</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>3.44893213700452</v>
+      <c r="C4" s="7" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" s="7" t="n">
+        <v>4.1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,214 +588,214 @@
         <v>36.2656384942249</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>2011</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="n">
-        <v>4.3042115113822</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>3.86078862247114</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>3.52181785867911</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>3.48932616727598</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>3.58515671200473</v>
-      </c>
-      <c r="H8" s="5" t="n">
-        <v>2.98867552929591</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <v>7.13069844140646</v>
-      </c>
-      <c r="J8" s="5" t="n">
-        <v>2.77560390254083</v>
-      </c>
-      <c r="K8" s="5" t="n">
-        <v>3.90033576054394</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="7" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="K8" s="7" t="n">
+        <v>4.4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>2011</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7" t="n">
-        <v>26.7344705254123</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>24.2578439824808</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>30.9303337909576</v>
-      </c>
-      <c r="F9" s="7" t="n">
-        <v>25.9386030072195</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>30.5211413364873</v>
-      </c>
-      <c r="H9" s="7" t="n">
-        <v>33.3653372722797</v>
-      </c>
-      <c r="I9" s="7" t="n">
-        <v>16.737592425129</v>
-      </c>
-      <c r="J9" s="7" t="n">
-        <v>42.2810038086294</v>
-      </c>
-      <c r="K9" s="7" t="n">
-        <v>27.2854976858582</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="n">
+      <c r="C9" s="8" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>30.9</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>25.9</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v>33.4</v>
+      </c>
+      <c r="I9" s="8" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="J9" s="8" t="n">
+        <v>42.3</v>
+      </c>
+      <c r="K9" s="8" t="n">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
         <v>2016</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="n">
-        <v>44.1</v>
-      </c>
-      <c r="D10" s="6" t="n">
-        <v>50.2</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v>34.7</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>43.9</v>
-      </c>
-      <c r="G10" s="6" t="n">
-        <v>38.7</v>
-      </c>
-      <c r="H10" s="6" t="n">
-        <v>36.4</v>
-      </c>
-      <c r="I10" s="6" t="n">
-        <v>50.3</v>
-      </c>
-      <c r="J10" s="6" t="n">
-        <v>18.3</v>
-      </c>
-      <c r="K10" s="6" t="n">
+      <c r="C10" s="9" t="n">
+        <v>36.8</v>
+      </c>
+      <c r="D10" s="9" t="n">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="n">
+      <c r="E10" s="9" t="n">
+        <v>29.3</v>
+      </c>
+      <c r="F10" s="9" t="n">
+        <v>31.8</v>
+      </c>
+      <c r="G10" s="9" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="H10" s="9" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="I10" s="9" t="n">
+        <v>44.6</v>
+      </c>
+      <c r="J10" s="9" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="K10" s="9" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
         <v>2016</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="D11" s="5" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="E11" s="5" t="n">
+      <c r="C11" s="7" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>32.7</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="G11" s="7" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="I11" s="7" t="n">
         <v>29.2</v>
       </c>
-      <c r="F11" s="5" t="n">
-        <v>22.6</v>
-      </c>
-      <c r="G11" s="5" t="n">
-        <v>27.8</v>
-      </c>
-      <c r="H11" s="5" t="n">
-        <v>25.8</v>
-      </c>
-      <c r="I11" s="5" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="J11" s="5" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="K11" s="5" t="n">
-        <v>25.7</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="n">
+      <c r="J11" s="7" t="n">
+        <v>41.6</v>
+      </c>
+      <c r="K11" s="7" t="n">
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
         <v>2016</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5" t="n">
-        <v>4.32751816114979</v>
-      </c>
-      <c r="D12" s="5" t="n">
-        <v>3.58533104925637</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <v>3.78103513077314</v>
-      </c>
-      <c r="F12" s="5" t="n">
-        <v>3.58546881803209</v>
-      </c>
-      <c r="G12" s="5" t="n">
-        <v>3.86334457621586</v>
-      </c>
-      <c r="H12" s="5" t="n">
-        <v>2.86601438591788</v>
-      </c>
-      <c r="I12" s="5" t="n">
-        <v>6.12129950885414</v>
-      </c>
-      <c r="J12" s="5" t="n">
-        <v>3.21581354182033</v>
-      </c>
-      <c r="K12" s="5" t="n">
-        <v>3.91930102547508</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="n">
+      <c r="C12" s="7" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G12" s="7" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="J12" s="7" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="K12" s="7" t="n">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
         <v>2016</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7" t="n">
-        <v>25.2</v>
-      </c>
-      <c r="D13" s="7" t="n">
-        <v>23.6</v>
-      </c>
-      <c r="E13" s="7" t="n">
-        <v>32</v>
-      </c>
-      <c r="F13" s="7" t="n">
-        <v>29.7</v>
-      </c>
-      <c r="G13" s="7" t="n">
+      <c r="C13" s="10" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="D13" s="10" t="n">
+        <v>26</v>
+      </c>
+      <c r="E13" s="10" t="n">
+        <v>33.6</v>
+      </c>
+      <c r="F13" s="10" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="G13" s="10" t="n">
+        <v>32.9</v>
+      </c>
+      <c r="H13" s="10" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="I13" s="10" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="J13" s="10" t="n">
+        <v>44.3</v>
+      </c>
+      <c r="K13" s="10" t="n">
         <v>29.3</v>
-      </c>
-      <c r="H13" s="7" t="n">
-        <v>34.6</v>
-      </c>
-      <c r="I13" s="7" t="n">
-        <v>17.8</v>
-      </c>
-      <c r="J13" s="7" t="n">
-        <v>41.5</v>
-      </c>
-      <c r="K13" s="7" t="n">
-        <v>27.1</v>
       </c>
     </row>
   </sheetData>
@@ -785,10 +814,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -799,23 +828,23 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -823,7 +852,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1" t="n">
@@ -831,44 +860,50 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="53.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="13" t="s">
+    <row r="8" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11"/>
+      <c r="B8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11"/>
+      <c r="B9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>